<commit_message>
Atualizações gerais no site: estilos, páginas da secretária e SQL
</commit_message>
<xml_diff>
--- a/Nova pasta/Backlog priorizado.xlsx
+++ b/Nova pasta/Backlog priorizado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\bruno\TCC\Nova pasta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C43FA4B-A3D5-4EC5-A565-9F512BD8D81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFD77C9-A225-485F-9C50-6D7D1E77CBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10590" xr2:uid="{46B93E44-AEDB-442F-BA9D-58764F7EE564}"/>
   </bookViews>
@@ -260,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,10 +302,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF26F068-7B84-4E2F-AE2F-E58343777516}">
-  <dimension ref="B2:N75"/>
+  <dimension ref="B2:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +641,7 @@
     <col min="14" max="14" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -839,9 +838,7 @@
       <c r="F8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="15">
-        <v>6</v>
-      </c>
+      <c r="H8" s="15"/>
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="2:14" ht="60" x14ac:dyDescent="0.25">
@@ -860,12 +857,10 @@
       <c r="F9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="16"/>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>
-      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
@@ -873,7 +868,6 @@
       <c r="D11" s="3"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
@@ -881,7 +875,6 @@
       <c r="D12" s="3"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
@@ -889,7 +882,6 @@
       <c r="D13" s="3"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
@@ -897,7 +889,6 @@
       <c r="D14" s="3"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
-      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
@@ -905,7 +896,6 @@
       <c r="D15" s="3"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
-      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
@@ -913,190 +903,24 @@
       <c r="D16" s="3"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
-      <c r="H16" s="16"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="16"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
-      <c r="H18" s="16"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
-      <c r="H19" s="16"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
-      <c r="H21" s="16"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
-      <c r="H22" s="16"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="16"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H25" s="16"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="16"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H27" s="16"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H28" s="16"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H29" s="16"/>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="16"/>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H32" s="16"/>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H33" s="16"/>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H34" s="16"/>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H35" s="16"/>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H36" s="16"/>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H37" s="16"/>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H38" s="16"/>
-    </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H39" s="16"/>
-    </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H40" s="16"/>
-    </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H41" s="16"/>
-    </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H42" s="16"/>
-    </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H43" s="16"/>
-    </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H44" s="16"/>
-    </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H45" s="16"/>
-    </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H46" s="16"/>
-    </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H47" s="16"/>
-    </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H48" s="16"/>
-    </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H49" s="16"/>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H50" s="16"/>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H51" s="16"/>
-    </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H52" s="16"/>
-    </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H53" s="16"/>
-    </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H54" s="16"/>
-    </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H55" s="16"/>
-    </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H56" s="16"/>
-    </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H57" s="16"/>
-    </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H58" s="16"/>
-    </row>
-    <row r="59" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H59" s="16"/>
-    </row>
-    <row r="60" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H60" s="16"/>
-    </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H61" s="16"/>
-    </row>
-    <row r="62" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H62" s="16"/>
-    </row>
-    <row r="63" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H63" s="16"/>
-    </row>
-    <row r="64" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H64" s="16"/>
-    </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H65" s="16"/>
-    </row>
-    <row r="66" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H66" s="16"/>
-    </row>
-    <row r="67" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H67" s="16"/>
-    </row>
-    <row r="68" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H68" s="16"/>
-    </row>
-    <row r="69" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H69" s="16"/>
-    </row>
-    <row r="70" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H70" s="16"/>
-    </row>
-    <row r="71" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H71" s="16"/>
-    </row>
-    <row r="72" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H72" s="16"/>
-    </row>
-    <row r="73" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H73" s="16"/>
-    </row>
-    <row r="74" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H74" s="16"/>
-    </row>
-    <row r="75" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H75" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>